<commit_message>
Guard 캐릭터 추가 + Sting_Collider 추가
</commit_message>
<xml_diff>
--- a/Assets/Data/Excels/Ability.xlsx
+++ b/Assets/Data/Excels/Ability.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TowerOfInfinity\Assets\Data\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA1F12D-160A-475E-AEDC-4D5CA3D887ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC77DAD1-1C41-4A6B-B98D-4C41C1AF4D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32130" yWindow="3195" windowWidth="21600" windowHeight="12405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -112,6 +112,13 @@
   </si>
   <si>
     <t>WEAPON_ARROW</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WEAPON_STING</t>
+  </si>
+  <si>
+    <t>BE_STING</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -440,7 +447,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -532,6 +539,20 @@
         <v>20</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>50003</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>51000</v>

</xml_diff>